<commit_message>
Get daily reddit data: Tue Feb 25 08:11:18 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_03_02.xlsx
+++ b/data/collected_data/2025_03_02.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C512"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3593 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1ixpu22</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>How to make nails grow in nice shapes?</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ixpu22/how_to_make_nails_grow_in_nice_shapes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1ixpj49</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Putzin around, can't sleep,it's too loud and colorful!!</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixpj49</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1ixp79a</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Why does my finger look like this? it’s</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixp79a</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1ixp04n</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>matcha nails I received lately💚what do you think?</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixp04n</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1ixoni8</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Hope you guys like it. 🙏🏽</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k81g12olc8le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1ixoefu</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Press/glue on nails</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixoefu</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1ixo7ap</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>which shape and color(s) suits my hands best?</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixo7ap</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1ixnmg9</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>polka dots make me happy</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixnmg9</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1ixnk0o</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>What size would be best for these press ons?</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixnk0o</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1ixndim</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Does anyone know why the white part starts so low down on my pointer finger?? Can i do anything to change it🥲🥲</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/haeq0a1ey7le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1ixmngq</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>My valentine inspired nails!</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixmngq</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1ixn68s</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Feb. nails</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cbf4es6bw7le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1ixm76g</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Does this break Overlay Rules?!</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ixm76g/does_this_break_overlay_rules/</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1ixlz6j</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Aqua mood</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixlz6j</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1ixls00</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Am i a victim of MMA?</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ixls00/am_i_a_victim_of_mma/</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1ixlize</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Say NO to DIP Nails &amp; Nail Dremels!</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ixlize/say_no_to_dip_nails_nail_dremels/</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1ixlk4g</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Did my favorite chrome color for the first time in a while :)</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hmsgnwujg7le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1ixljii</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>is it embarrassing to anyone else to get their nails done?</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ixljii/is_it_embarrassing_to_anyone_else_to_get_their/</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1ixlepn</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Finished my first full set on myself!</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zsphnl98f7le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1ixl6u9</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Can I still wear Christmas colors in February?🥺</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j1hyc3j8d7le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1ixkx70</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Rings of fire?</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xekla72ua7le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1ixkexy</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>builder gel over gel polish??</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ixkexy/builder_gel_over_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1ixjk1n</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Nails for tomboy w/dermatillomania</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2quy2mixy6le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1ixk1x6</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Variety Nail Polish (Regular and Gel)</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ixk1x6/variety_nail_polish_regular_and_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1ixjpfk</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>I can’t turn back after first Russian</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xr10od9707le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1ixj4v6</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>What's the best Mani technique to get the most natural looking nail extensions?</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ixj4v6/whats_the_best_mani_technique_to_get_the_most/</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1ixisof</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Press ons by my bsf&lt;3</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixisof</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1ixilic</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>What do they look like?</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixilic</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1ixidly</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Wedding nails. Exactly like my reference pic, they turned out perfectly</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixidly</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1ixi2zj</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Is it giving cat eye?</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jyuthkc4m6le1</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1ixi1qp</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>How to remove dried polish from sweater?</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixi1qp</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1ixhzz4</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>first time doing soft builder gel on myself!</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bf73451jl6le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1ixg7ql</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Can I glue on gel nails if I have an allergy?</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ixg7ql/can_i_glue_on_gel_nails_if_i_have_an_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1ixg55q</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Preventing nail thinning with press ons? (press on application help)</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ixg55q/preventing_nail_thinning_with_press_ons_press_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1ixhlf0</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>How do they stick their crystals so that they last a long time?</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixhlf0</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1ixh7dc</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>I did these myself!</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5m33qg03f6le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1ixh6m9</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Butterfly Nails 🦋</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixh6m9</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1ixh5cj</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Decided to go pink this time</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r5a0ecmne6le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1ixgjzb</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Which nail shape and length would look best on me?</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixgjzb</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1ixgftz</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Press on set I made just in time for cake day!!</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixgftz</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1ixg8rc</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>not the neatest work, but i’m getting there!</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixg8rc</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1ixg5y6</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>My first ever gel polish at home</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixg5y6</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1ixfwtm</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>I would wear milky white everyday for the rest of my life😍</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/831r7iku46le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1ixfs4j</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>First try French tips??</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixfs4j</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1ixfn1p</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>back again with more outgrown nail pics 🙃</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixfn1p</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1ixfbex</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Swampy moldy psychedelic</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2kuiy6gd06le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1ixf38p</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>I'm learning acrylic so fun</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixf38p</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1ixf2ku</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>is it normal for my BIAB nails to grow this much after 2 weeks?</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jnmflxriy5le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1ixenc0</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Little beetle moment</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixenc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1ix87vs</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Gel X nails popped off</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ix87vs/gel_x_nails_popped_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1ixaz57</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Gel X Question</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixaz57</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1ixef5k</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Got my nails done in Japan!</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9p3k9vfrt5le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1ixedkn</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Almond or coffin nails?</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixedkn</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1ixe3qk</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>New favorite GelX</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oeu1knfir5le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1ixdcaz</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>More gel, or grow out first?</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bwu05wtwl5le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1ixcum4</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>What to do?</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6r0ebcefi5le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1ixcptp</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Beetles nail</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ixcptp/beetles_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1ixcwbo</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Chrome Nails - Love Shiny Sets 🦋🩵💜</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixcwbo</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1ixcseo</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Tried something new - not sure if i like them 🧚</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qdlzsslzh5le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1ixcs7g</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Black, love 🖤</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gilcwruxh5le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1ixc9b0</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>b-day nails ☺️</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixc9b0</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1ixc5t1</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>My pretty nails, and question for shape</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixc5t1</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1ixbsfv</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Plus Life Lacquer - Train Graveyard 🚂 🪦</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixbsfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1ixblg8</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>i’m obsessed with my new nails c:</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixblg8</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1ixbigi</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Is this color acceptable for mid thirties and am I doing anything wrong?</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ilsjvkqs85le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1ixbfbc</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>More sparkly nails 💅</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixbfbc</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1ixb8ex</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>My nails!!!💅</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixb8ex</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1ixb4yb</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Does this nail length and shape suits me?? ( I do my own nails,if you can't tell haha)</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ons1axe365le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1ixb2e3</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Asked her to do some trippy nails and she killed it</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cal47uyk55le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1iwzuyp</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Why is my builder gel so sheer at the free edge? Any tips for this?</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zhcg8hjsn2le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1ixabpe</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>new set in a loooong time</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixabpe</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1ixa9ur</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>All things fake nails</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ixa9ur/all_things_fake_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1ixa3gg</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Spring swan 🦢</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iou7gd5ly4le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1ixa22g</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Is builder gel supposed to be this far from my cuticle?</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/txbf7px9y4le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1ix9ouq</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Velvet nails ✨💅🏾💙</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2tqlgj4nv4le1</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1ix01ut</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Regular nail polish on top of gel</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ix01ut/regular_nail_polish_on_top_of_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1ix94bm</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>idk what it is about a fresh gel mani but I feel so slay rn</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ix94bm</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1ix8zyz</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Monday Mani ( Black /White</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k9qg78pfq4le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1ix8m8o</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>3rd time doing my own acrylics at home</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ix8m8o</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1ix8jb0</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>BIAB on natural nails ~ still having a moment for gold accents</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ix8jb0</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1ix7be6</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Visions inspired nails</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ix7be6</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1ix7e5c</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Why this excessive pain😓</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ix7e5c</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1ix7tka</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Brittle nails</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ix7tka/brittle_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1ix89yw</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Cat eye w/gold 3d art</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ix89yw</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1ix7zd1</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>perfect combination</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5a3260cdj4le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1ix7l01</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>What do you think about that decision?? Is it look nice?</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ix7l01</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1ix7k7l</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Is it therapeutic for you too?</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ix7k7l/is_it_therapeutic_for_you_too/</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1ix7dgx</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Damaged nails and home polish</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2exe2wu0f4le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1ix6ys7</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>New set I did! What do you think?</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ix6ys7</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1ix6p8f</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Does this shape suit me?</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7zq20ek8a4le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1ix6k8b</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>I still get I sessed every time I get them done. No one believes me when I tell them these are my natural nails!</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9si3cj6994le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1ix6h7b</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>St. Paddy's Day set!</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3r7yptyn84le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1ix69hc</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>magnetic gel in the morn 💕</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ix69hc</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1ix15bx</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Advice please after bad mani</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9b4lb72r13le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1ix2xh0</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Based on my nails, what are your suggestions for a clean at home mani?</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ix2xh0</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1ix2zae</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Can regular nail polish ever look as good as gel nails etc?</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ix2zae/can_regular_nail_polish_ever_look_as_good_as_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1ix4x7h</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Is it possible to have nails done long-term without damage?</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ix4x7h/is_it_possible_to_have_nails_done_longterm/</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1ix4s62</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Self gel manicure questions</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ix4s62/self_gel_manicure_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1ix5ufz</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Reflective mani!!</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ix5ufz</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1ix5tex</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Purple Chrome On Black 🔮</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rpkwv9op34le1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1ixpch3</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Consumerism</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ixpch3/consumerism/</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1ixp5ot</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Not a fan of white mani but this one's an exception</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k73m55yqi8le1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1ixoinu</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Watch Your Sanity</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixoinu</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1ixodad</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Should I use a nail hardener?</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ixodad/should_i_use_a_nail_hardener/</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1ixnb6k</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>OPI Infinite Shine - how different is the formula?</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ixnb6k/opi_infinite_shine_how_different_is_the_formula/</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1ixmwls</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Clover - ILNP</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qfq0c3oit7le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1ixmg5c</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Purple Skittle</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixmg5c</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1ixmfmg</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>I see you Dollar Tree!</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixmfmg</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1ixlynn</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Flower Child appreciation post</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixlynn</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1ixlqkg</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>✨New Kozmic Colours Polishes Review✨</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l03kk915i7le1</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1ixl41y</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>EdM skittle!</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixl41y</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1ixl3pt</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>LynB/ILNP skittle!</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixl3pt</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1ixkm9p</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Holo Taco Fifty Shades of Greige🩶✨️</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixkm9p</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1ixkf9g</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Confetti, Set, Go!</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cv8vnlrf67le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1ixkeze</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Clionadh - Gorgeous to behold impossible to photograph</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jme7nhnc67le1</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1ixjqbs</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>EdM’s Always Around Me is mesmerizing ✨</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixjqbs</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1ixjenu</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>ILNP Eclipse - need an all teal dupe</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o4zdnnvlx6le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1ixj7rf</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Kbshimmer's Spring Collection Delayed</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m4gdk1exv6le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1ixj4e7</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>What's the best Mani technique to get the most natural looking nail extensions?</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ixj4e7/whats_the_best_mani_technique_to_get_the_most/</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1ixim5z</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Help healing damaged nails from picking?</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixim5z</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1ixib4h</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Different Lightings, One Stunning Polish</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixib4h</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1ixhvi7</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Looking for a way out</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixhvi7</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1ixhj8u</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Alien Life Form</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixhj8u</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1ixgybt</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Glowy polish to beat the gloom</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixgybt</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1ixgxit</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Fierce Mojo💜</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lh8h3vluc6le1</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1ixgvn1</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Pack of gel polish</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ixgvn1/pack_of_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1ixgt1p</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Update: shade matched my donkey, thanks!</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k7ubm9qvb6le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1ixggjw</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Freaking out... Do I have greenies?</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixggjw</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1ixgdj7</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Mood: Quite Literally Dead Inside</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f2u043k286le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1ixgcv4</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Hard gel popping off on one finger only</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ixgcv4/hard_gel_popping_off_on_one_finger_only/</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1ixg68u</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>help on shaping curved natural nails into almond shape</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixg68u</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1ixg63f</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Vampy polishes for pale pink skin?</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ixg63f/vampy_polishes_for_pale_pink_skin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1ixevh2</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Zhulong</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixevh2</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1ixedbi</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>thaaat's better. when u redo ur mani after less than one hour...</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixedbi</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1ixe65t</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>can’t stop taking pictures of my nails…</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixe65t</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1ixe3gg</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Obsessed with House of Hades</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9pje4megr5le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1ixdskt</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Looking for a dupe for this colour 🍊</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3i6bp5q8p5le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1ixdloy</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>I made this!!!!! 🤩🤩🥳🥳💅</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixdloy</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1ixd6sc</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Zoya “Happi” and ILNP “Karma”</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ad93ta9tk5le1</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1ixcsvl</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Does anyone else not magnetize their magnet polish?</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ixcsvl/does_anyone_else_not_magnetize_their_magnet_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1ixcq8a</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>there's a subtle purple shift, so pretty!</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixcq8a</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1ixcnwu</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Are ridges and peeling nails due to nail products?</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/71yrdmo1h5le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1ixcbee</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Gold &amp; Green</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixcbee</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1ixbtsb</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>My first post here as a newbie to nail polish</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixbtsb</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1ixbtga</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Plus Life Lacquer - Train Graveyard 🚂 🪦</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixbtga</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1ixbbe8</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>sh insta dri syrup polishes</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2kobdjke75le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1ixb6y5</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>desperado under the stars</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixb6y5</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1ixb0nm</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Polished For Days - Eternal Glow</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixb0nm</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1ixakko</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>4 Hours</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixakko</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1ixaecj</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>How long does a WBTC take to dry?</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixaecj</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1ixa9bn</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Do you ever go through periods where you don’t feel interested in polishes anymore?</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixa9bn</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1ixa0rz</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Waiting for Spring</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixa0rz</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1ix9z7w</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Sunstone/Moonstone</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ix9z7w</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1ix9ytm</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Pure Magic ✨️</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3mre7zgmx4le1</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1ix8zf2</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>My fav shade to use in between winter &amp; spring 🥹💙</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ix8zf2</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1ix8s0k</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Spring is coming</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ix8s0k</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1ix81r9</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Pisces Season ♓️ Mani</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ix81r9</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1ix7zee</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Thank you to poster who inspired me to polish my nails more in 2025</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ix7zee/thank_you_to_poster_who_inspired_me_to_polish_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1ix7yau</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Green of Mermaid Bait?</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bp07ksy5j4le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1ix7u0w</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>First go at watermarbling</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ix7u0w</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1ix7cwm</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Not sure if I like this polish but I can’t stop staring at my nails</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ix7cwm</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1ix6qzd</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Fall Leaves Skittle in Winter! 🍂🍁</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/10snoe6ma4le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1ix6p4n</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>shooting star in the sun 🌞🌠</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d2eujit8a4le1</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1ix6l65</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>✨Embracing darker colors this week✨</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ix6l65</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1ix6i1u</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Finally nailed the chrome polish technique!!</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ojmzm6u84le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1ix6hdy</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>I truly cannot buy any more polishes right now 😫</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ix6hdy</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1ix6dw0</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Clionadh’s Pastel Yellow?</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/on49e7dx74le1</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1ix66d2</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>🍜</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ix66d2</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1ix5qna</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>It's giving Mardis Gras vibes</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t4c7bix534le1</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1ix5qq8</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>when the polish barely matches the pics online… then you get a chip on day 1 and decide it’s coming off ASAP 🤬</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ix5qq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1ix5fzz</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>I just can't get over this one</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lvtz8xq014le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1ix5cmm</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Influence / De-influence me on Cirque Midsummer Night</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m8m1omke04le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1ix4swy</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Nocturne Ritual</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ix4swy</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1ix4col</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Can you help me identify this Orly polish?</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ix4col/can_you_help_me_identify_this_orly_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1ix37bv</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>👍😝Most Used Emojis🌈✨️</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ix37bv</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1ix2ien</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Sunday Mani showoff</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lrelwvb2e3le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1ix2886</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>imperial stormtrooper 🖤🩶</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ix27ug</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1ix0tyd</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>I understand the hype now.</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ngg8a33jy2le1</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1ix0ttq</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Heavenmetal 🌌✨️</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ix0ttq</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1iwzic6</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iwzic6/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1iwz2nx</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>When in doubt, pink holo</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o2nddghbe2le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1iwxujp</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Is clear polish or base/top coat better to protect my nails from water?</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iwxujp/is_clear_polish_or_basetop_coat_better_to_protect/</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1iwx55c</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Ready for spring 💐</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iwx55c</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1ixpxl0</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Cherry Nails</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixpxl0</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1ixpj2s</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>I'm so happy with how this turned out! Hand painted this myself :)</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixpj2s</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1ixoza3</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>First time doing intricate isolated chrome and rhinestones!</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w8aygg0lg8le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1ixof78</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Chrome Nails</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixof78</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1ixmr6c</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>I chose a lilac dress for my birthday and want to get almond-shaped long nails. But I can’t decide on the color. I’m torn between ecru, pink, and a lilac shade that matches my dress. Which one do you think I should go for?</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ixmr6c/i_chose_a_lilac_dress_for_my_birthday_and_want_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1ixks4z</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>MPA x NarinaChan "The Artist Palette" Review</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixks4z</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1ixkpz6</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Learning to work with gel polish.</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ykajxnq297le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1ixj8kd</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Coraline Nails 🪡</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n3wny4b4w6le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1ixfo9n</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>back again with more outgrown nail pics 🙃</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixfo9n</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1ixfapa</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Swampy moldy psychedelic</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t0uyvl6806le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1ixb7p8</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Alien vs Predator set</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixb7p8</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1ix9gtp</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Pink animal print! Cute right?</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m3i6fol2u4le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1ix95an</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Made my first press on set :)</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ix95an</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1ix83ir</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>My first attempts at painting nail art</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ix83ir</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1ix7o6y</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Love playing with chrome and cateye together!</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ix7o6y</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1ix74cx</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Created a set that’s out of my usual style, unsure on them 🫤</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oxd3f825d4le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1ix5ybj</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>First press on set!</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wj0bkaht44le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1ix4jk1</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Beautiful, all hand-drawn</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1l2xwnjbu3le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1ix4glz</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>IDK how to pose my hands. I had to leave my V-Day appointment with unfinished nails &amp; had to finish them myself.</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/axpyk62pt3le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1ix4clt</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>My newest set done by my queen @nails_emmywynn on IG</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fqlb9n8us3le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1ix48s4</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Some cat eye florals and chrome, love them!</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tus80jymr3le1</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1ix39rj</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>3 sets of press ons I made, I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ix39rj</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1ix2f8x</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Favorite time of year is almost here! The green season!</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ngwuk45bd3le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1ix1l0k</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Psychedelic.. Pretty?</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ihzrkxyv53le1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1ix0wjg</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>What u think about it ?? My first nail art trial</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zozbu5x9z2le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1iwxpq6</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Tried some Pinterest inspo nails</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/43dj8197x1le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1iwgvwr</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>My pink nails for March</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lrqz6awymxke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1iwj4mo</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Thoughts? 🤔 (Nails done by me)</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iwj4mo</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Feb 26 08:11:24 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_03_02.xlsx
+++ b/data/collected_data/2025_03_02.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C512"/>
+  <dimension ref="A1:C690"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9137,6 +9137,3032 @@
         </is>
       </c>
     </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1iyijnv</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>matching sets :)</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3vemj6vaxfle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1iyhqxz</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>well this just happened...😭</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a4pseshzmfle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1iyh9xi</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>nails design set for a client 🖤</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyh9xi</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1iyh84l</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Not ready to give up wintery blues, but I'm excited for spring! Swipe for step-by-step process</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyh84l</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1iyg1y7</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>3rd time doing GelX on myself</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kdqlzehm3fle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1iyftqh</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Retro manicure and pedicure</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyftqh</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1iyfqf3</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>I’m so obsessed with these</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/daqliqkf0fle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1iyfbdw</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Got pink and red nails for an upcoming winery trip 🍷</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/saqkcp9zvele1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1iyf0un</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>In search of TikTok press-on nail creator!</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iyf0un/in_search_of_tiktok_presson_nail_creator/</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1iyet4w</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Got my nails done for my birthday!</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyet4w</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1iyenjh</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Spring Nails</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2b1g7nskpele1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1iyel9y</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>I broke a nail😪</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/umphug5zoele1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1iyeget</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>; do these look like press ons?</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyeget</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1iye4fq</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Nail color suggestion</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lect5ighkele1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1iye45p</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>It’s giving galaxy Barbie? Idk but I’m in love 😍</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iye45p</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1iye25a</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Cherries 🍒</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iye25a</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1iydzfq</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Hard gel overlay in Houston?</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iydzfq/hard_gel_overlay_in_houston/</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1iydphw</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>bday set!</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o9hm0vymgele1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1iydoo7</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>my attempt at French tips</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iydoo7</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1iydmpv</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Nothing better than a fresh set 💅</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ga1w8n6yfele1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1iydi6m</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Gelx set I did</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/93733tbseele1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1iyddbv</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Recent set!</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyddbv</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1iydb5x</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Eye see you..</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t5yi7910dele1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1iyd4fr</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Eh?</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyd4fr</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1iyd3gq</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Olive&amp;June red velvet nails❤️</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyd3gq</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1iyd2ot</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Chocolate 🍫</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ig1w8wnuaele1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1iycl0n</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Can I paint over T.A.P. gel?</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iycl0n/can_i_paint_over_tap_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1iyccoc</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>How do I apply cuticle oil🤦‍♀️</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iyccoc/how_do_i_apply_cuticle_oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1iycalt</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Starter kit for gel nails</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iycalt/starter_kit_for_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1iyciep</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Newest set</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/offpxgrv5ele1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1iybtle</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Watermelon ombre vibes!</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pe3js4xqzdle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1iybs2a</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>First time I’ve gotten the pearl/chrome dust on my pink white ombré.  I’m a big neutral nail girl but wanted sparkle✨</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iybs2a</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1iybia5</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Flores 💐</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dq2j8yv2xdle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1iy8rbt</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Home vs salon gel manicure</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iy8rbt/home_vs_salon_gel_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1iy5hk4</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Should I get a fill?</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/clyhtzsrlcle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1iy9cba</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>At Home Nail Recs Needed!</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iy9cba/at_home_nail_recs_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1iyb2gs</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Went with square shape nails this time because they’re easier to play video games with 🥹</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyb2gs</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1iyax7o</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Frenchies with a twist 🤍⚜️</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m3f9l4pyrdle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1iyaqxm</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Wishful Spring-Thinking Nails</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/medy5mehqdle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1iyahvm</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Finally got my isolated chrome technique down</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7y85n9nfodle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1iya0by</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>For nail techs, have you all ever questioned if this career is right for you or not?</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iya0by/for_nail_techs_have_you_all_ever_questioned_if/</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1iy9t7g</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Can yall post your current sets in the caption?</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iy9t7g/can_yall_post_your_current_sets_in_the_caption/</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1iy9glc</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>At Home Nail Recs!</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iy9glc/at_home_nail_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1iy8hl2</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Round or Almond?</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy8hl2</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1iy7jsz</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>My favoritest ever!</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy7jsz</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1iy7zc3</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>I think it's very elegant</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zdqfdqua4dle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1iy7udj</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>What do you think of my nails? I think they're pretty!</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy7udj</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1iy7tzo</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Would you get this set?</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy7tzo</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1iy7okq</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Starry Nails</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy7okq</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1iy48jr</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>What I Wanted Versus What I Got</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qd8vtp0kccle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1iy7f9o</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Polygel confetti</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy7f9o</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1iy7ak5</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Help me get better at doing my gel nails!!!</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nan0jnp1zcle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1iy76t5</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Should you put top coat on press on nails?</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iy76t5/should_you_put_top_coat_on_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1iy6ylz</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Pink holo nails</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/49tn8e3mwcle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1iy6ite</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Today is blue</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z3xtfmmdtcle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1iy6bc5</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>What can I say....I love glitter</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy6bc5</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1iy5yzg</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>What do you think of the nail stickers?</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy5yzg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1iy5lfv</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>My latest French set with a twist</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy5lfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1iy5i3c</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>🫧</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy5i3c</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1iy5g20</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>A subtle change into Spring 🌷</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mso8kzmglcle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1iy5ft3</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Tangled nails!</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy5ft3</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1iy59gn</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Got my nails done last night love them but they are already chipping..can I go get them fixed without feeling dramatic?</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy59gn</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1iy51mx</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Cat eye obsession. I couldn't choose a color, so it's different on both my hands</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy51mx</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1iy4u14</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Saw a new nail tech today, she did NOT disappoint 🍃</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy4u14</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1iy478f</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Bikini bottom nails</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy478f</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1iy43th</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Lavander💜</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wpxut63kbcle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1iy3n7l</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>I love blooming gel</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/okerx8868cle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1iy3lt1</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>I did my own chrome nails for my trip 🏝️</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy3lt1</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1iy33c5</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>My newest set</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy33c5</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1iy2q3l</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Please help</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy2q3l</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1iy2www</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Breakfast at Tiffany’s 💅</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/42x08izq2cle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1iy2wgv</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>New Mails 💝</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/urwfvm3o2cle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1iy2j42</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>All my previous sets were $100+</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy2j42</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1iy2d69</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>simple but cute nude/ burgundy nails</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i8qzmeityble1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1ixvsyk</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>How do I prevent this/clean it before curing?</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ct09ardolale1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1ixzpxk</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>New to Nails... What to Do Next?</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ixzpxk/new_to_nails_what_to_do_next/</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1ixwwwb</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>There are so many options I don't understand what to get.</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ixwwwb/there_are_so_many_options_i_dont_understand_what/</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1iy0odb</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Staying safe at nail salon?</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iy0odb/staying_safe_at_nail_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1iy21zd</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Just for fun!</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jr0q6lzkwble1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1iy1a9k</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>trying to conjure spring vibes here in the uk!</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/355gh762rble1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1iy14fj</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Here to brag about my nail artist 💅🏼</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lz3bzwxvpble1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1iy0zy3</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>This month's mani</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qh40jrxyoble1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1iy0hvs</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>She never fails to amaze me.</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy0hvs</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1ixzdyi</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Cracked down the middle</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixzdyi</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1ixxr9h</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>This week’s Mani</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixxr9h</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1ixvtwq</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Embarrassed to get Pedicure</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sou5eajwlale1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1ixzmdg</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>pink + chrome biab!</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gh84ets0fble1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1ixykc8</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Question for contact wear</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ixykc8/question_for_contact_wear/</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1ixy0of</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Holographic Nails //</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/af64jbn43ble1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1ixx618</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>What can be upgraded?</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6bd965xkwale1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1ixx5dg</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Thin french tips look good ?</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lpf0z1mgwale1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1ixwzxd</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Have to get better at taking pics</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ozm2h3xavale1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1ixvz47</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>A purple kinda day 💜</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixvz47</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1ixvirn</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Second time I've ever had an oval done! I love it! Also, this color is such a match for my cat!</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixvirn</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1ixvh97</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Time for a colour and shape change</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixvh97</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1ixumh9</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>new week new nail polish</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pbvzactlbale1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1ixuleq</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>solution to stop biting my nails</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ev4bshb8bale1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1ixud75</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>It's so beautiful and elegant</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/66d8tmo49ale1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1ixu0l4</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>simple gel nails to commemorate my 3year work anniversary!</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xvebdqot5ale1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1ixtso9</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Russian Manicure</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ac9108o3ale1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1iyheu2</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Has anyone tried polishes from Fauve cosmetics?</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iyheu2/has_anyone_tried_polishes_from_fauve_cosmetics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1iyg5s8</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>What is this in my new bottle? Mold?</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyg5s8</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1iyfbq3</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Is there a way to make fake tips look good with just polish?</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iyfbq3/is_there_a_way_to_make_fake_tips_look_good_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1iyf0pm</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Devil's Advocate vs Read vs Complimentary Wine</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iyf0pm/devils_advocate_vs_read_vs_complimentary_wine/</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1iyexqj</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>First attempt at nail art!</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyexqj</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1iyedxd</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Clionadh Cosmetics Oxidize</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyedxd</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1iydp5t</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Jury 🌹⚖️🪨 Nullification</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iydp5t</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1iydhjz</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Pow!</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iydhjz</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1iydh3s</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Treehouse is the sleeper hit of my ILNP order</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iydh3s</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1iyd94p</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Fake halo is that gorl</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e2j9eyhhcele1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1iycw46</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>The many faces of Forbidden Desire</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iycw46</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1iycvsc</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>foiled!</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iycvsc</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1iycmw3</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Nail polish color?</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ve2dcnzx6ele1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1iybdm7</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Pacific Northwest /Twilight vibes</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iybdm7</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1iyb7q7</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Holo Taco Wild Child and Garden Party Taco</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyb7q7</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1iy9esq</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Way beyond my comfort zone</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy9esq</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1iy93kb</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Tried the glass nail look by u/Icouldmaybesaveyou and I think I might never take it off</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j77jcywncdle1</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1iy8yib</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Handmade Gel Press-On Nails Question</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iy8yib/handmade_gel_presson_nails_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1iy8uch</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Spring green holo</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy8uch</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1iy83o7</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Me: "oh shit, gotta be out the door in 5 mins but my nails are nude". This single-coat baddie: "I gotchu 😘"</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dvwflbl85dle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1iy7mwl</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Battle of the beetles? What are your favorite oil spill/beetle-esque polishes?</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/drr1y16n1dle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1iy707a</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>OBSESSED</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ixhody8ywcle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1iy5wkx</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Matching nails with my LO</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy5wkx</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1iy5ppz</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Metal &amp; magnet tip!</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pspytlufncle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1iy5cj8</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Does moat method damage nails?</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy5cj8</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1iy4wy6</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Unicorn Dreams by Inspired Sense</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy4wy6</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1iy4mg8</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Has anyone received their January LBOH order yet?</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iy4mg8/has_anyone_received_their_january_lboh_order_yet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1iy4d2j</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Help choosing between Mooncat polishes</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iy4d2j/help_choosing_between_mooncat_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1iy3y96</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Solar + Thermal = 👀👀👀</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy3y96</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1iy3n72</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>help me with my PFD cart!</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy3n72</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1iy37ql</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Had to stop my run to capture this polish</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy37ql</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1iy2nnw</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Found the Perfect Non-Streaky White Nail Polish</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rjq3qzeq0cle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1iy2l3h</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Holo taco cold slate, NailsInc rocket fuel for some ✨sparkle✨, and a nosy cat!</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ydft44e0cle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1iy2cw8</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>I wore this on a trip to the Arctic and the color changes were so entertaining</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5vxnv2w6yble1</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1iy1yfe</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Obsessed with this New Magnetic Effect</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1nln0h1svble1</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1iy1igz</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>my year in nails so far</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy1igz</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1iy0rvq</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Is Cirque Colors available in Canada?</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy0rvq</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1iy0q70</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Baby's first flakie</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy0q70</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1iy0k84</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>ILNP Deep Space lives up to the hype 💫</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/60n9dxdulble1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1iy0dos</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>It’s Only Magic</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy0dos</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1ixywdi</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>DIY peely base</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ixywdi/diy_peely_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1ixyvwf</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>[ISO] Panda Painter 2.0 Dupe</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wnyn61xl9ble1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1ixyu2l</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Pool party VS Blue Rizzler?</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ixyu2l/pool_party_vs_blue_rizzler/</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1ixxgh3</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Purple Polish</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixxgh3</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1ixx31n</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>✨️🩵Teal Gradient🩵✨️</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixx31n</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1ixx1pk</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>9 whimsical nail polish shades💅</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixx1pk</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1ixwdxf</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Need this shade!</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mgtfmhshqale1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1ixw8xn</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>if you saw my post from yesterday… new ILNP manicure to replace the disappointment that was Cirque pipe dream.</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixw8xn</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1ixw81j</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>When you can’t resist a sunny mani pic!</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ovbh425pale1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1ixvkob</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Time for a colour and shape change</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixvkob</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1ixvkfg</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Galaxy 🌌</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixvkfg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1ixus6b</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>I get why people love thermals now</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixus6b</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1ixlxup</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Aqua mood</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixlxup</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1ixt42e</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Confused between BIAB/builder gel vs acrylics?</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ixt42e/confused_between_biabbuilder_gel_vs_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1ixt4of</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Metallic lilacs as in Mooncat TMTYL base</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/43djc5wmw9le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1ixsufl</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>I had a nightmare about ILNP</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ixsufl/i_had_a_nightmare_about_ilnp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1ixsem0</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Naturally pink</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixsem0</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1ixrytf</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Daiso ❤️ Nail wraps</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixrytf</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1ixrj21</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>“It’s ‘DIGNITY’ Luanne!”</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/db3lokamd9le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1ixrc5y</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>would you believe these are extensions? hard gel is the dream! nails by me (__kmnails)</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6btuut87b9le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1ixr01k</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>How do you make good pics of glitter nails?</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixr01k</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1ixqlu9</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Broke a nail and had to go short, but at least I have pretty polish to soothe my emotional wounds</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2sy8q8zl19le1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1iyffpl</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>I painted my pets on my nails because I miss them 🥺</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyffpl</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1iyf89l</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Valentina❤️</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyf89l</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1iyemka</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Spring Nails</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fpyl4zhbpele1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1iye5mm</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Cherries 🍒</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iye5mm</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1iydn6s</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Gel nail art</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1iydn6s/gel_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1iyb9ue</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Gel polish problem?</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1iyb9ue/gel_polish_problem/</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1iyb5kr</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>On myself ❤️ second set ever!</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyb5kr</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1iyavtp</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Wanna try nail art but no clue where to start.</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1iyavtp/wanna_try_nail_art_but_no_clue_where_to_start/</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1iy6tiv</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>silent hill-themed shorties</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy6tiv</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1iy5a4l</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>New pose for me, what do we think ??</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ledjyv58kcle1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1iy2pho</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Still trying to learn but feeling good about this weeks nails</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fnf3ocpa1cle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1iy1b9d</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Getting better at my straight lines :))</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s3iipyu8rble1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1iy0k3n</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>This week’s Mani</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iy0k3n</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1ixuwiw</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Blue fires</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e19vigy2eale1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1ixr69f</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Chunky Nails</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ixr69f</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1ixqeq7</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Green fairy 🌿🧚✨</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cw8hy0wyy8le1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Feb 27 08:11:14 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_03_02.xlsx
+++ b/data/collected_data/2025_03_02.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C690"/>
+  <dimension ref="A1:C873"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12163,6 +12163,3117 @@
         </is>
       </c>
     </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1iz9psn</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Accidentally gave myself Thanos-inspired nails</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uhx8byddomle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1iz9qu2</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Making nail polish last</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iz9qu2/making_nail_polish_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1iz81gk</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Help Severe nail peeling</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iz81gk</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1iz9dom</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>leopard print + pink nails &gt;.•</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iz9dom</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1iz8z8a</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Why is a classic red the best nail colour</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u1qokfklfmle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1iz8ru7</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Baddie nails 🍒🔥💅🏼</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mcqdx5vadmle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1iz8hx6</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>chrome gel mani</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iz8hx6</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1iz7kk4</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>The longest I had my natural nails</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tgohxe5m0mle1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1iz7f14</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Springish Set. 🐄</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d48gkru2zlle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1iz7cag</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Some of my recent favorites 💅</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iz7cag</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1iz78vs</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Desperate for purple glitter</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iz78vs/desperate_for_purple_glitter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1iz6la6</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>SOS</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gtjq96nxqlle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1iz62j4</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Cat eye</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tu3dpe0zllle1</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1iz5tnr</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>very beautiful and nice</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ou8bebvsjlle1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1iz4o6e</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Is my nail lifting?</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iz4o6e</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1iz5kfk</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Press On Girlies 💅🏼</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iz5kfk</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1iz4z2s</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Nails for a Car Show</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iz4z2s</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1iz4uyu</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Curved nails</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iz4uyu/curved_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1iz4u3x</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Unexpected Matchy Matchy</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iz4u3x</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1iz4om4</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Thoughts on this brand for flat bail beds</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gfx2hb8d9lle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1iz4gyh</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>💕✨</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v1om6ete7lle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1iz461e</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Am I just not supposed to use my hands? (press-ons)</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iz461e/am_i_just_not_supposed_to_use_my_hands_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1iz3w5t</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>new set, made by me</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/klm4ssr72lle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1iz3r47</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Finally finished Nina from Creature Commandos!</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fzjeqjh21lle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1iz2l1x</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>What do I do to heal this?</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z0a40cr1rkle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1iz1ovr</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>I tore off my gel polish and now my nails really sting</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iz1ovr/i_tore_off_my_gel_polish_and_now_my_nails_really/</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1iz30ot</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Funky cow nail art I did 🥰</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lnza49zqukle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1iz2yg8</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>New spring nails I just did!</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iz2yg8</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1iz2uc3</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>First Builder Gel Attempt!</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iz2uc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1iz2t7m</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>I made them for the 14th, what do you think? ☺️</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ga8rt12zskle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1iz2o2s</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>ISO: An indestructible manicure (or as close as I can get to one)</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iz2o2s/iso_an_indestructible_manicure_or_as_close_as_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1iz2jpf</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>something clean and bright for incoming spring :-)</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/koqewxdqqkle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1iz1pmy</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Free service, how much do I tip?</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iz1pmy</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1iz1gn4</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Some questions about nail strengthener</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iz1gn4/some_questions_about_nail_strengthener/</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1iz1b0c</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>HEMA free press on nails/ Acrylic free press on nails</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iz1b0c/hema_free_press_on_nails_acrylic_free_press_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1iyzls5</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>How to remove acrylic nail with a break?</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iyzls5/how_to_remove_acrylic_nail_with_a_break/</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1iz1ch2</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Just started doing my own gel nails</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iz1ch2</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1iz1b3m</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>I just realized I matched my nails to my water bottle</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iz1b3m</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1iz18q3</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Sparkly pink</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iz18q3</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1iz0vw8</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Non acrylic/ Hema free press on nails</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iz0vw8/non_acrylic_hema_free_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1iz129o</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>New nails 😍</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iz129o</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1iz0vk2</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Paint stroke</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iz0vk2</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1iz0th4</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Spirited Away soot sprite nails</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iz0th4</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1iz03uw</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Baby blue</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9w9axrdy6kle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1iyzxk5</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Two sets I did this week</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyzxk5</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1iyzi0x</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Can I use semi cured gel strips with nail extensions?</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iyzi0x/can_i_use_semi_cured_gel_strips_with_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1iyzet9</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Is this my soap nail color?</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyzet9</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1iyz36f</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Mica powder question</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iyz36f/mica_powder_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1iyxw2q</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>$25 mani- thoughts?</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dp35y7bcqjle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1iyxsfx</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>I'm so in love with my nails rn 🥰 this colour is part of a new range at my local nail salon</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j28vfjgkpjle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1iyxqn6</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>DnD Dark teal with Ibd hard gel base.</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qnvd6d57pjle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1iylsud</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Can anyone tell me why some of my nails are pushing back like this on my pinkie and ring finger?</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ttl2wdvp2hle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1iywzsk</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Painted my nails for the first time in a while</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/00lo1zpmjjle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1iywxer</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>My Nail Journey</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iywxer</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1iywx5u</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Fresh set on point</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ucde9z2jjle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1iyws1l</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Help! Lifted nail bed</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyws1l</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1iywr1i</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Barbie Beverly Hills Fashions set</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iywr1i</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1iyw43g</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Can you show me nails that are trendy for 2025 or that are youthful? I feel stuck in the same style</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lijl3oe2djle1</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1iyvqtr</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>My natural nails with a thin layer of clear gel</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/me1fwzsdajle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1iyvjqz</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Mica powder</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iyvjqz/mica_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1iyvjpl</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Blue at the Botanical Gardens ♡</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xw271q0y8jle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1iyv8at</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>🤍💚✨️🏵</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tt6sxjuo6jle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1iyv2z3</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>white french tips ❤️</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fq64lhml5jle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1iyv12v</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Pepto pink clouds 💖</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eld805p75jle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1iyuobt</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>French tips on top of leopard print?</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/amdlyqrl2jle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1iyu2px</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Press on help</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xj8z7wmayile1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1iyu1xb</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>February Nails</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyu1xb</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1iysqgd</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Are you supposed to wipe inhibition layer after every application?</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iysqgd/are_you_supposed_to_wipe_inhibition_layer_after/</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1iytqag</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Content recommendations please!</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iytqag/content_recommendations_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1iyt4t6</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>I messed up - beginner mistakes.</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyt4t6</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1iyta0b</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Long red coffin shaped: iconic for a reason</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyta0b</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1iyt88l</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Recently been experimenting with press on nails, here are some of my favorites from this month</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyt88l</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1iyt3xb</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Need a bit of help with my press ons.</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyt3xb</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1iysvp8</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Valentine Nails</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6d283z2npile1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1iysr9t</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Strawberry Nails</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iysr9t</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1iyspqr</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Rainbow cateye flames</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyspqr</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1iysoyb</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Coworker said I’m not showing enough skin. Are my press ons too close to my cuticles? (tw: partial amputee)</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iysoyb</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1iysoat</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>gel at home</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iysoat</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1iys9eo</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Are you feeling it?</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/aux78ve7lile1</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1iyof41</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>What's wrong with my nails?</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bsswhrmirhle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1iyo4b5</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Am I being too picky?</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyo4b5</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1iyju0s</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Very damaged nails</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyju0s</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1iyq7nf</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Nail detached BIAB HELP</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iyq7nf/nail_detached_biab_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1iynb8v</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Cat’s eye never gets old!</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iynb8v</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1iymvdw</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Nude polish is my favorite</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xdyqhuikdhle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1iyl791</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>girl. what is this i’m freakin owwwwt :(</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyl791</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1iykren</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>I got my nails done for the first time ever (in a salon)!!</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iykren</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1iykg2w</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Newbie nails</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ylri9fzjmgle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1iyi5ri</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Minor onycholysis on pinky; help!</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iyi5ri/minor_onycholysis_on_pinky_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1iyhct8</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>What helped your nails grow stronger, longer, and healthier? Please share your must-have products and go-to routines?</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iyhct8/what_helped_your_nails_grow_stronger_longer_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1iyrnlh</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>They're very far from perfect, but I'm proud of them!</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyrnlh</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1iyrm4j</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Special Mother/Daughter nails for adoption day 🥰</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1svg52qcgile1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1iyrbhb</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Left hand actually turned out better :O</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyrbhb</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1iyr2gf</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>MOONCAT - Full Scream Ahead</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyr2gf</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1iyqinv</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>This blue hue neon green is so fun</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lg6n3jma8ile1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1iyqbhs</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Creamy nude with some texture ✨</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyqbhs</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1iyq8rk</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Soft and dainty</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p8avsrd66ile1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1iypm9l</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>we have the power when we do our nails✨ confirm that ✨</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hm9zhkja1ile1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1iyph0v</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>It’s summer in my country, so I painted my nails in summery colors ☀️</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p3qvp1w50ile1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1iyp0s3</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Just a Trans Woman excited to Show off my new sparkly gray nails</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyp0s3</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1iz8zz1</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Cooties by Death Valley Nails 🤩</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iz8zz1</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1iz8ffb</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Fridge magnet collection swatches</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vn9lh5hh9mle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1iz6pkc</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Looking for a dupe</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ixhouph4slle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1iz6nq2</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>ILNP Annabelle</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iz6nq2</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1iz6is0</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Trying the new magnet technique from earlier</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r99nyjboplle1</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1iz6fa1</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Milky ombré shorties</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iz6fa1</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1iz5ltq</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Mooncat and ILNP combo</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iz5ltq</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1iz5cci</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Blue Kind Of Day</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yadrkxgeflle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1iz4v4j</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Found an old box of nail polishes</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iz4v4j/found_an_old_box_of_nail_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1iz4k59</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Favorite I’ve done on my nails so far 😍</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iz4k59</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1iz3p9l</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>the most beautiful jelly berry magenta for a dress photoshoot 🍒🍓</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iz3p9l</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1iz3f9u</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Can anyone recommend a white, black, and clear (not top coat?) polish that is specifically good for water marbling? Noticing how some brands are simply not ideal for this technique!</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f71mdgmyxkle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1iz3c67</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>First Time Stamping How’d I Do? 🫣</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ybue3ongxkle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1iz383v</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Allegic reaction</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iz383v/allegic_reaction/</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1iz31ms</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Swatched my entire collection!</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iz31ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1iz2q1a</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>ORLY Bonder Damage or something else?</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x8zmjbt7skle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1iz2ox7</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Cirque Starry Eyed</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iz2ox7</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1iz1zww</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>It’s giving space galaxy Barbie 💅</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iz1zww</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1iz1xnh</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Skittle of… whatever this is, my new color fixation</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l0wsysfllkle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1iz1mga</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>One True Love</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iz1mga</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1iyzzsk</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>🌬From Air to Sea🌊</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyzzsk</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1iyzo5u</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Replacement lid for Night Owl bottles that fit Indigo Bananas brushes?</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iyzo5u/replacement_lid_for_night_owl_bottles_that_fit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1iyyzb1</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Why does kbshimmer’s qdtc smell like that??</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iyyzb1/why_does_kbshimmers_qdtc_smell_like_that/</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1iyyvoy</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Matchy matchy with my gear!</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyyvoy</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1iyybpo</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>February Manis Collection</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyybpo</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1iyyb5l</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Finally did my nails after 3 weeks, cannot video for nuthin' 💖💚</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cciewv2ftjle1</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1iyy6yh</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Shifty shades will always have my heart</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j0sc0i6ksjle1</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1iyxyuw</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>anyone else use their nails as a dopamine hit during the day? 🥲</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyxyuw</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1iyxkmm</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>DVN stay a while</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyxkmm</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1iyxcgd</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Something a bit more subtle* today</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9cdbgyi9mjle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1iywzat</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Fun with nails 💅</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iywzat</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1iywqkb</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>had to do a big chop so i did a treat myself polish!! 🪻🪻</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iywqkb</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1iywmh1</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Angels Flight to Starry Nights by OPI is a dreamy sky blue nail polish with an oh so subtle holographic rainbow finish. 😇🌟</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iywmh1</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1iywa82</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>First timer need gel removal advice!</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bduyyy5cejle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1iyvzlr</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Does anyone else’s nails look like this when you remove polish?</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0gn6cce5cjle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1iyvsh7</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Accidental Photoshoot</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyvsh7</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1iyu3ff</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Linear Holo skittle for Spring 🩵</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyu3ff</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1iytuhf</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>help find a polish with these two colors</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iytuhf</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1iytj72</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>VERY new to nail care - what do I do?</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iytj72/very_new_to_nail_care_what_do_i_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1iytgdi</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>update with “response”: cirque polish doesn’t match their pics online</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iytgdi</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1iyssts</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Base Coats, Your Favorites and why?</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iyssts/base_coats_your_favorites_and_why/</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1iysrg4</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Deep blue sea 💙</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tngktxssoile1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1iysgtv</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Um, Amazon?</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/30td3njomile1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1iysd6z</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Trying glitter polish for French Tips😻</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ou575wmulile1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1iys6rz</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Is this a dupe for PFD goblins and ghoulies?</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0un4enmnkile1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1iyri23</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>ILNP killing it with the jellies</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ac3hzojfile1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1iyr7x2</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>My very greedy mani (I want everything on my nails!!!)</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mgnw9fufdile1</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1iyr2xu</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>MOONCAT - Full Scream Ahead</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyr2xu</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1iyqhs1</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>She wore pink velvet...</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xfr0sk348ile1</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1iyq1gd</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Shleee Polish's 'Escapism'</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyq1gd</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1iyplij</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Is Canmake any good?</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iyplij/is_canmake_any_good/</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1iypgxx</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>How about some color to brighten up those winter days? 🌈✨</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iypgxx</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1iypf0g</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Looking for a mini set of pastels!</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iypf0g</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1iyp3jp</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Is it giving Mardi Gras or Halloween?</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyp3jp</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1iyp31e</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>🤎🧡70's Carpet🧡🤎</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyp31e</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1iyoquz</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>In my cateye era</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vogs2kj7uhle1</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1iyo6i7</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Essie Romper Room 🩷</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b8rgo0fiphle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1iynxp3</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>This is the most gel-like magnetic I've ever seen! Absolutely incredible</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1rh8ythanhle1</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1iylro6</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Managed to save polish from a dropped Mooncat bottle (clumsy AF)</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iylro6</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1iyjrlr</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Seche vive alternative?</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iyjrlr/seche_vive_alternative/</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1iyc6av</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Pink Shimmer Comparisons</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyc6av</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1iyg6hx</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Deep Space by ILNP 🛸</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iyg6hx</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1iyjbz5</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Tequila Sunrise anybody? 🍹</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/whhsgytr7gle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1iza2mx</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Neon Halloween set 🕷️💀🎃</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iza2mx</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1iz9zy7</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Life is not perfect....</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6xcs1txxrmle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1iz9xef</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Beginner</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1iz9xef/beginner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1iz77dx</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Fishing lures nails</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iz77dx</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1iz52os</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Bubble Nails</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h3lqwnnyclle1</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1iz3qml</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Finally finished Nina from Creature Commandos!</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/brjfsocy0lle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1iz3473</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Koi nails</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iz3473</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1iz325n</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Started with a rose petal and then it kinda got away from me</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/udx6rlc3vkle1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1iz24j5</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>New stuff ✨💅🏼</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iz24j5</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1iz230k</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Going big or going home</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iz230k</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1iz1sof</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Nail design help</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ixiimhwfkkle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1iz0uwx</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Paint stroke</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iz0uwx</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1iywu82</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Made myself some birthday nails</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/67ngu8zgijle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1iywt0u</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Barbie Beverly Hills Fashions set</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iywt0u</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1iyti89</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Pink will always be my color of choice</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q30f5t16uile1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1iysvoi</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Preserving my bouquet!</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iysvoi</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1iys5sx</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Painting Gels Recommendations..</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1iys5sx/painting_gels_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1iyqp1l</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Got custom nail stickers of my bbys!!</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vowc2arl9ile1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1iynwst</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Buen día que les parece este</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ocdek9j6nhle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1iylqvn</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Light, airy and incredibly feminine</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g7dvaij02hle1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Feb 28 08:11:06 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_03_02.xlsx
+++ b/data/collected_data/2025_03_02.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C873"/>
+  <dimension ref="A1:C1050"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15274,6 +15274,3015 @@
         </is>
       </c>
     </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1j029r5</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Do you do a fresh set of nails every time you change designs?</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j029r5/do_you_do_a_fresh_set_of_nails_every_time_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1j0284l</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>deep V-cut french with peach chrome &lt;3</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0284l</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1j01q2k</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>I painted a shoebox to hold my nail essentials!</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fkquozr9utle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1j0198m</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Help me theme my nails!</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j0198m/help_me_theme_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1j00mpj</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Rate this out of 10</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j00mpj</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1izz71f</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Glass file ruining nails, what do I do?</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izz71f</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1j009lv</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Blueberry Milk</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j009lv</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1j000xl</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>🔮</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j000xl</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1izzih1</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Any ideas for a color like this?</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y709zcqd5tle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1izyxo4</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>My current set</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izyxo4</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1izytg2</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Suggestions?</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1izytg2/suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1izynvd</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Ready for spring🌷🌸</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izynvd</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1izy9kg</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>First time tying gel x</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ia7bbocxssle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1izy6ug</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Learning</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izy6ug</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1izxrf5</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>are these too thick?</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izxrf5</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1izxzyy</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Sheep nails 🤍 hoo</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izxzyy</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1izx584</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Contact dermatitis????</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izx584</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1izxjia</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Periwinkle Blue</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yjcqkfvylsle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1izx1nk</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Anybody have luck using builder and/or top coat on top of press ons to help with durability?</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izx1nk</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1izx185</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>I know there are many that hate mixing press ons with gels… what about bartbox which is apparently designed to work with gels?</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izx185</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1izwx1i</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>One year without, my baby's is back!</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izwx1i</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1izwumf</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Luv owls 🦉❤</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izwumf</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1izwkpa</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Best Builder/Rubber Base Gel?</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1izwkpa/best_builderrubber_base_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1izvyxc</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>it’s hard to do anything with these … but they look amazing</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izvyxc</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1izvq2z</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Nude almond-ish shape on natural nails</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fo60k1x05sle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1izvm15</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Frequently Broken Nail</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izvm15</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1izvb8p</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>best nail shape for me?</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izvb8p</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1izva2f</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>A SHORT OVAL RUSSIAN GEL MANICURE W A FRENCH TIP 🤍</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lhtsa78z0sle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1izv0sx</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Vocaloids as Chibi Nail Art!</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izv0sx</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1izuzzg</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>I'm 16, this is my first time trying to put glue om nails on myself. Does the way they're put on look weird?</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izuzzg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1izudwk</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>I love my nails 😍</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ostro8ebtrle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1izslwj</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Chrome nails on white gel?</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1izslwj/chrome_nails_on_white_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1izszp8</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Dyeing my nails with Jagua</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izszp8</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1izt3cv</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Overgrown hyponychium</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gpybugahirle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1izttl2</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Refilled nails. Is the base color ok?</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t4uaofxforle1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1izszu2</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>What am I doing wrong?</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/472pfmxohrle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1izsdhd</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>"Fingerless Glove" Nails?</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izsdhd</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1izs8eb</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>almond or coffin on me?</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izs8eb</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1izs5hj</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Sort of a rushed job today... But I love that the color matches my tumbler speckles ☺️</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izs5hj</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1izrwbk</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Misshapen nail from writers bump- advice on reshaping??</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izrwbk</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1izrngb</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Nails + Baby</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1izrngb/nails_baby/</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1izs2ur</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>what’s your favorite base color or combo for a french tip?</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1izs2ur/whats_your_favorite_base_color_or_combo_for_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1izryzq</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Polish turning grey??</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izryzq</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1izrozx</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>My basic set with a little razzle dazzle😭</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/040cohpe7rle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1izrnpq</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>‘Spotted’ my next great success! ♥️🐆</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izrnpq</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1izrm27</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Acrylics</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1izrm27/acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1izr81h</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>New Set 🥳🍒🤍</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y2al6j0s3rle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1izr80l</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>What color to choose?</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n8r8opxr3rle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1izqi27</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Tried nail art for the first time pls tell me your thoughts!</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izqi27</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1izqbx0</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>French press-ons!</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izqbx0</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1izq89r</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Didn't realize how long my natural nails had gotten</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7mmbv387wqle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1izq6tp</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Does this shape complement my hand or do I need a different shape?</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dcimkdnvvqle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1izpvk5</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>I love my new nails</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2jxjfffgtqle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1izpsyz</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Cat’s eye love it got them done today :)</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izpsyz</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1izpoyw</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>I live in North York Ontario. Do you guys know any good nail salons in my area? If so who would be the nail tech you'd recommend to go to? Thanks for your help. ❤</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1izpoyw/i_live_in_north_york_ontario_do_you_guys_know_any/</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1izpmae</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>What’s happening to my nail polish???</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izpmae</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1izpi0o</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>First cateye nails</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ygb76p5mqqle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1izp5k6</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>freestyle nail forms i did on my friend 🖤</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izp5k6</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1izp1wb</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Fun with gel liners and magnetics</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vxtpzv04nqle1</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1izp1pk</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Category is: Mediterranean 🍊</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z6ap8ec6nqle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1izom4v</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Ready for blue skies 🩵</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izom4v</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1izoin2</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Nail Strengthener</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1izoin2/nail_strengthener/</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1izohm5</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Acrylic nails removal is this normal ?</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izohm5</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1izofnz</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>New shape and length wanted!</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/481478vjiqle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1izoct5</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Mineral bond treatments?</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1izoct5/mineral_bond_treatments/</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1izo9kz</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Tried a neutral and not disappointed 🤍</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ui62vxa9hqle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1izo4e3</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>OPI mod about you 💕🌸🎀🌷</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izo4e3</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1izo02h</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Did I ask for colored acrylic wrong?</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1izo02h/did_i_ask_for_colored_acrylic_wrong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1izno4c</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>My first Spring set of the year (press on)</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kp6xfabucqle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1iznnuu</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Black &amp; gold ⚜️</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wy8eaz6scqle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1izngg6</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Which nail shape/length looks best with my hands?</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izngg6</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1izn3j8</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>What is the blue liquid they soak your feet in at a pedicure?</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1izn3j8/what_is_the_blue_liquid_they_soak_your_feet_in_at/</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1izmnz3</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Will my nails ever heal? Skin picker.</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izmnz3</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1izmgy4</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Sally Hansen cuticle remover</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1izmgy4/sally_hansen_cuticle_remover/</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1izf9hr</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Help deciding!</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/22kcn9gckole1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1izadr5</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Bio Sculpture Lamps</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1izadr5/bio_sculpture_lamps/</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1izdbh9</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Can someone please ELI5 why i should opt for BIAB over other gel types?</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1izdbh9/can_someone_please_eli5_why_i_should_opt_for_biab/</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1izhxxg</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>So apparently, if my nails are more red and marbly-looking, they’re OVERFILED which is WRONG?!</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izhxxg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1izi872</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>please help me find a lasting gel polish</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1izi872/please_help_me_find_a_lasting_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1izlqem</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Accidentally matched my PS5 controller</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izlqem</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1izgg75</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Advice for chronic nail biter?</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1izgg75/advice_for_chronic_nail_biter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1izldfx</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Porcelain nails</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izldfx</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1izi8wn</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Cut near nail</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1izi8wn/cut_near_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1izl24b</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Nail tech used dremel on my cuticles question..</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rmtai61stple1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1izabp8</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>How do I prevent this?</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zkw3uon8wmle1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1iza19p</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Recommendations for press-ons</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iza19p/recommendations_for_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1izi0e6</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>need help!!! natural nails on the brink of death</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ny70tuy97ple1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1izdqyo</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Which kind of nail do I get?</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1izdqyo/which_kind_of_nail_do_i_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1izif5p</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>PlEaSE help me find a lasting gel polish 😭😭</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1izif5p/please_help_me_find_a_lasting_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1izkry6</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>What should I do?</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izkry6</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1izkn9a</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Acrylic overlays, new set or infills?</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1izkn9a/acrylic_overlays_new_set_or_infills/</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1izj0d6</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Did gems and pearls for this set. First time using something that needed to be glued on!</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izj0d6</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1izixbd</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>natural set 🤍 retention prep practice</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izixbd</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1izivld</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Jem - Shana Elmsworth</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izivld</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1izijfi</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>What is the best shape on me?</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izijfi</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1izif47</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>A bit late but here’s the Valentines nails I had!!</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xzxdtlhgaple1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1izi4r3</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Help me figure out what’s off</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bbetr7i88ple1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1izi07l</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>✨Good morning! What do you think? It's another cute set, right?</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/whbk4ow87ple1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1izhyti</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>best nail shape?</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izhyti</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1izhy27</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Are Glamnetics Press-On-Nails worth it? (+ Question about Press-Ons)</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1izhy27/are_glamnetics_pressonnails_worth_it_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1j0245x</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>How to velvetize with bar magnets?</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8jg1h9e6ztle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1j01p0u</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>I painted a shoebox to hold my nail essentials!</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2u5dxrnwttle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1j00f04</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>I tried the new magnet trick🪄🧲</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ul818k60ftle1</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1izz7ou</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Cirque Paradox</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ndoprbc2tle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1izyf8j</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Clionadh Psilo siblings trio!</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izyf8j</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1izyb1l</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>A Terrible Price</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m6g8f1ibtsle1</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1izxduz</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>New favorite prop.</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izxduz</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1izx7av</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Shorty creme</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izx7av</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1izwpna</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>New magnetic 🤩</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izwpna</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1izvmzk</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>OPI Gemini and I</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xr85puo84sle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1izvkt3</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>my first Emily de Molly 💗</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izvkt3</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1izuy1l</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>BKL freebies?</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1izuy1l/bkl_freebies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1iztwqh</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Reverse velvet with bar magnets?</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iztwqh/reverse_velvet_with_bar_magnets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1izt6im</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>a combo I didn’t know I needed</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izt6im</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1izsg1a</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>ISO Gemstone-y nail polishes!</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izsg1a</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1izrqsa</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>In my flakes era</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izrqsa</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1izrq2x</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Advice on timing Pedi😩</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1izrq2x/advice_on_timing_pedi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1izrhx5</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>help me not ruin my nails plz!</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1izrhx5/help_me_not_ruin_my_nails_plz/</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1izqysg</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>I can't stop staring at them every possible lighting</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izqysg</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1izqt8s</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Kintsugi inspired set!</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w5l3xlem0rle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1izqh02</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Just a Trans Woman excited to Show off my new sparkly slate nails</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izqh02</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1izqa09</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>When your polish matches your book…</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izqa09</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1izpznd</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>NCT concert nails 💚🥳</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izpznd</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1izpym7</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Base Coat Recommendations</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1izpym7/base_coat_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1izpv3z</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Are you ever just enthralled by your own nails?</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izpv3z</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1izpgyw</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Engaged in Polished for Days 💅🥰</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izpgyw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1izpcfc</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Not bad for a $3 polish from Walmart</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izpcfc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1izoqul</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Lavender Syrup - Holo Taco</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izoqul</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1izombm</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>To Yeild More Than One Molecule</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izombm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1izoh7r</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>My happy little heart 🙌</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i9vriplwiqle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1iznsv5</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Having a bad day</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iznsv5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1izmab6</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>What Mooncat Green Eyed Monster should look like?</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/it3lq7sq2qle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1izm4lv</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Behold: The Magnet Holder</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wqe2n7il1qle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1izm0hq</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Holo Taco Emerald City Dupe?</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ihjj00u0qle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1izlz82</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>I have officially peaked as a lacquerista!</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ronk414k0qle1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1izle3x</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Bring it, Spring. Looking at you, purple Irises</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/axvkfu66wple1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1izl2yp</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>BKL Snake</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x7gvehtxtple1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1izky19</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>the difference between direct and indirect sunlight 😮‍💨</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izky19</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1izku8z</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Feeling Blue</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izku8z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1izkpil</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>🎵 I’m a sucker for you 🎵</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izkpil</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1izklqd</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Have y'all ever injured your nails?</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1izklqd/have_yall_ever_injured_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1izkc53</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Clove oil safe for daily use? 🤔</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1izkc53/clove_oil_safe_for_daily_use/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1izk2b5</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Blue and teal mani</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izk2b5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1izjs7r</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Peachy goodness</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2n58kwghkple1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1izj2g7</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>great lakes lacquer hype?</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1izj2g7/great_lakes_lacquer_hype/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1izisda</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Take Me to Your Leader 👽</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izisda</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1izinca</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Vintage brooch inspired nail art 🌿🌸☁️</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izinca</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1izifkx</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Looking for a red/orange chunky glitter polish</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a04vlasjaple1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1izi0n4</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Strawberry pink nails 🍓</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izi0n4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1izhuel</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>🌟🎈Lucky Charms🩷🧲</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izhuel</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1izhojw</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>What is the effect on the right hand  and how do I do it? Is it possible to do it with regular polish?</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mpmzw8pp4ple1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1izh73x</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>✨Fancy Fingers✨ BURBERRY</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3byxvm5o0ple1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1izgcvh</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Anchor &amp; Heart hiatus</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1izgcvh/anchor_heart_hiatus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1izg2uu</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Their Polish Calls to Me Like Green Goblin's Suit: Fauve Cosmetics</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izg2uu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1izfrk4</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Does anyone else refer to polishes as ‘her’?</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1izfrk4/does_anyone_else_refer_to_polishes_as_her/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1izf6hl</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Base Coat Battle Round 3! I’m</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izf6hl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1ized5b</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>ORLY “Serendipity”</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ized5b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1j020kb</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>freehand brushstroke</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/55d5ebyvxtle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1j01evg</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>What are Some Trendy Nail Art Designs that Every Girl Loves?</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1j01evg/what_are_some_trendy_nail_art_designs_that_every/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1j00iz7</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Found embellishments in the craft section, Fruity!</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j00iz7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1izyh7o</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Hello Kitty glam nails</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izyh7o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1izyc3i</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Care bears x Lucky charms 🙈</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izyc3i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1izxsud</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Powerpuff girl 💖</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kj2kostgosle1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1izw2sc</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Shamrocks and stripes</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tu9nov298sle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1izv1hd</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Vocaloids as Chibi Nail Art!</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izv1hd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1izuh6p</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>I changed the flower because I didn’t like it 😌 swipe for the inspiration ✨</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izuh6p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1izu783</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>My nails and inspo 💅🏼</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izu783</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1izrkjk</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>My first set of 3D nails</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9m5lbnkg6rle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1izpubx</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Super Late Valentines Care Bears</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izpubx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1izo7z8</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Suggestions for wedding nails</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1izo7z8/suggestions_for_wedding_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1iznn9f</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Gold flowers 💛</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7a93iqtncqle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1izjdmp</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Disappointing apples 😅</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xmv2m20ihple1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1izj4hy</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>The set vs the inspo 🤍</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1izj4hy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1iziz5q</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Press on set I made for a friend who’s expecting a baby boy 💙</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r7n59jlleple1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1izhptb</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Green cat eye 😊</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4pgmljzy4ple1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1izg2ib</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Better Pic of junk nails!</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/82jqhh42role1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1izeuc5</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Junk chrome freestyle nails</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2z6uffd9gole1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Mar  1 08:09:39 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_03_02.xlsx
+++ b/data/collected_data/2025_03_02.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1050"/>
+  <dimension ref="A1:C1229"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18283,6 +18283,3049 @@
         </is>
       </c>
     </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1j0u78q</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Throwback to Christmas vibes</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8byv6bbj71me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1j0u4oq</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Which shape for my hands?</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0u4oq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1j0u3rn</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Red heart with silver swords and black elements ❤️⚔️🖤</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0u3rn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1j0tkk0</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>nosferatu nails at work :)</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b0ly8g2tz0me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1j0si28</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Spring nails</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ln0gi7en0me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1j0tacm</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>First time with 3D nails 💚🍀🐸</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0tacm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1j0sosa</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Seeking advice!</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j0sosa/seeking_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1j0swwr</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Natural Nails with Spring Theme!</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0swwr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1j0poqz</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>nail shape?</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0poqz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1j0pnx5</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Hello Spring! 🌷💐 Inspo: @bees.knees.nails on IG.</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lnh1muq5uzle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1j0o6b2</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Tried a new color: Mystic Marine</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0o6b2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1j0rilr</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>First time and I am in love 🥹💜🩷🩵💛</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mixaja5uc0me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1j0r68p</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>🎂🎀🎈Birthday Nails from last month! Such a fun set to make</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0r68p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1j0r5qe</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Slowly growing back 🤍</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r41t65s290me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1j0qz7h</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Any Natural Nail care tips</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0qz7h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1j0qp7z</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Feeling girly. 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p7zdsuid40me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1j0oayk</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Not sure what to do when builder gel grows out?</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j0oayk/not_sure_what_to_do_when_builder_gel_grows_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1j0ox8m</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Spring Nails, What I go vs what I asked for, inspo @elbebeauty on IG!</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0ox8m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1j0pwkc</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>First Ever Handmade Press Ons</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0pwkc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1j0pvce</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Felt like summer this week!</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nifvigj3wzle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1j0pule</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Which is flattering on me?</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0pule</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1j0pt79</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>New set I did with some stickers from Amazon</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ai11wovivzle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1j0p0zb</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Would you believe I paid 18 USD for this nails?</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8pf0oud2ozle1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1j0obyz</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>For the planets</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0obyz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1j0nvhp</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>my two favorite nail sets I've done for myself</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0nvhp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1j0nu3w</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>I’m ready for Spring!</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pzqrocftczle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1j0nti6</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Mardi Gras</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k69dmbsnczle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1j0nm77</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Was feeling WICKED 🪄🫧</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p4t7g3qtazle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1j0n1xm</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Two custom press-on sets from a seller on Etsy! Two of my favorite hobbies in one for the fountain pens, and I have a great love of L&amp;O.</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0n1xm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1j0mtr6</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>I feel like photos never capture the beauty in the polish. How do you guys take such pretty pics!?</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0mtr6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1j0mt9m</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>New press ons that i got today!</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5l2d6al3zle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1j0mqla</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Beginner at doing my own nails</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0mqla</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1j0l7i0</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Can someone tell me why every time I apply false nails, press ons, that only the thumbs split down the middle and the others are fine. I have to apply a fresh set after a week bc of this and the rest of the nails still look fab 😭. After they split they eventually break. Thank you!</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j0l7i0/can_someone_tell_me_why_every_time_i_apply_false/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1j0lbbu</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Did these for a friend's drag show!!!</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tdv9ch5vqyle1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1j0leaq</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>New jelly set with charms</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xrlkxttiryle1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1j0mntr</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Chrome hearts with gold jewellery?</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j0mntr/chrome_hearts_with_gold_jewellery/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1j0loo7</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Creoq eu me quedaron como el traste😢</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0loo7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1j0mdzu</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Obligatory Which shape suits me best?</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0mdzu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1j0lhrd</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>I’m new here, just got this done yesterday! 💕🔥</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ef9lb76dsyle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1j0ku3f</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>💥Stranger Things💥</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0ku3f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1j0ktme</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>just got my nails done for the first time ever and i’m obsessed</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tdwz8eivmyle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1j0krh8</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Too thick? Second time getting nails done</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0krh8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1j0kkf5</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Fun nail art ideas for girls night</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j0kkf5/fun_nail_art_ideas_for_girls_night/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1j0kcp4</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Nails are a disaster - these are filed way too thin, aren’t they?</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/55i8w465jyle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1j0hzlm</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Help to damaged nails. 🙏</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nhkia1al0yle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1j0jzyn</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>First DIY gel set ^.^</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0jzyn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1j0jwy8</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>they’re short but look so good with this effect (cat eye) 😻</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5e7kdrrnfyle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1j0jd9r</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>wanted to try something new and i love them. What do you think?</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0jd9r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1j0imsd</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Is there a difference between BIAB and strongbase ?</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zcbk4e875yle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1j0hrxm</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>🩷 Painted Polish pink crelly skittle for the last day of February 🩷</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jxogfj8xyxle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1j0fc2o</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Advice for nail supplies</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j0fc2o/advice_for_nail_supplies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1j0hii5</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>are these bad..</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ft3tw71wwxle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1j0gytj</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Help me pick!! Read first please! Press ons all from Etsy shops, none are mine, just shopping: 1) @SkyNailShop 2) @MythicalNailart 3) @DizzyMoonGift 4) @RadiantlovecreDesign 5,6,7) @hananailsart 8,9) @DizzyMoonGift</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0gytj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1j0hdzk</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Neutral nail color suggestions!</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gvk7p5kxvxle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1j0hcmn</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>How can I make my nails more well-groomed?</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/674rfmzmvxle1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1j0hc8k</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Gel overlay with my new nail stickers! ☺️</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0hc8k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1j0hbs1</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Loving This Color!</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0hbs1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1j0h986</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>🦋</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0h986</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1j0gkp0</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Spring nails</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/253jqklrpxle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1j0gjxc</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>SOS: Any suggestions?</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/36lisijlpxle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1j0gjq8</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>What do you think of my nails?</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pb71iexfpxle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1j0ge5b</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Time between new nail polish</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j0ge5b/time_between_new_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1j0g853</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>took me 4 hours!💅🏻</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0g853</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1j0g2in</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>I’m so happy with how these came out I worked so hard on them lol</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0g2in</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1j0fvf1</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>💙🦋🌀Ceramic Set</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8le2i6tekxle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1j0f6vy</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Tried the thermal by itself and wasn’t a big fan; threw some magnetic gel on top and now I’m in love 🥰</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xmbdpps2fxle1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1j0eyml</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Alternative ideas for this set by @serenadidem on Instagram</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gvv82qqddxle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1j0dmvb</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Never gotten nails done and don’t know what to ask for</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0dmvb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1j0e8bb</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>st patrick's day without being overtly st patrick's day</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0e8bb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1j0e3zx</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Chrome application</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j0e3zx/chrome_application/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1j0dpug</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>My nails</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0dpug</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1j0dgl5</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>How to manage nails that grow upwards</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cyfesyf72xle1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1j0dbjy</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>My nail guy is the best!!</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0dbjy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1j0csbt</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Any recommendations to strengthen my nails? They are too fragile and break easily.</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/899avas7xwle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1j0chhk</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>💅So Ladies let me know what you think, Also I’m going to show you a simple way to do your own nails that glue on. Cost is around 15.00 tops. Side note if you file to much remember to just apply another coat don’t touch up. Depending on the color you use.</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0chhk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1j0cf1h</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>My nail tech called me out for how long I take to pick a color. No regrets.</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f8etlkwkuwle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1j0c80q</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Ahh my nail tech is absolutely magical!! 🫶🏻💞</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0c80q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1j0alsc</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Most effective way to paint your nails?</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j0alsc/most_effective_way_to_paint_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1j0brmq</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>I did a new set!</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0brmq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1j08xjy</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>SOS- gel polish on top of builder gel not lasting</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j08xjy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1j04yjg</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Just took them off, miss these nails 💔</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j04yjg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1j0bgsa</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Getting nails done professionally for the first time</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j0bgsa/getting_nails_done_professionally_for_the_first/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1j0b8ly</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>What shape nail suits my hand best?</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0b8ly</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1j0b0b9</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>:((( idk how I feel.</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0b0b9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1j09war</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Pls rate my first ever free of charge service!</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pb49kt1zbwle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1j09qow</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>“Mommy, we do nail salon?”</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pwzr19wsawle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1j08kpq</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>did my own ladybug nails :P</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j08kpq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1j085n6</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Rate this? I definitely love this design, it’s elegant🎀</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rwy9x96txvle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1j0853q</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Cute bees</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0853q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1j07rgu</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Handmade Press-ons</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dmr6ij4euvle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1j07n50</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Salon etiquette?</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j07n50/salon_etiquette/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1j073q7</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Opinions? 👀</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7d9f2x0hovle1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1j06pa2</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Which repair product works better</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j06pa2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1j06dy3</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Tried something new</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/586xfydehvle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1j066hv</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>First time trying cats eye and I'm hooked!</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ryx8oid7fvle1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1j05czm</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>March set 🌈</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j05czm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1j04mv7</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>New BIAB set. Feels like a 90s kids birthday party vibe!</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t80ajlatwule1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1j044xr</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Can’t let go of the cherry fever.</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j044xr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1j042li</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>My nails that I did yesterday.</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j042li</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1j034w4</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Favorite valentines set</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sf2nacfqcule1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1j0unqa</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>A bit disappointed</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0unqa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1j0tjy4</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>When do you call it quits?</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ygo40snlz0me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1j0t9xx</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Glow in the Dark PINK nail polish topper? Or pink GITD polish??</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j0t9xx/glow_in_the_dark_pink_nail_polish_topper_or_pink/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1j0t9bu</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Forces of Evil❤️</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0t9bu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1j0slr6</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>✨layering✨</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0slr6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1j0r9n8</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Bravocado</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/eOmlfL1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1j0r8a9</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Batsquatch 🦇 🦧</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0r8a9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1j0q9t9</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>The sink after they shave</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0q9t9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1j0q41r</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>cock a doodle doom ❤️💜</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0q41r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1j0pchy</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>New Mooncat!</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0pchy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1j0oxjv</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Sour apple rings dupe??</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0oxjv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1j0oma0</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>I am once again jumping on the new magnetic technique bandwagon</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0oma0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1j0nwms</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Getting distracted on my walk (ILNP Shooting Star)</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0nwms</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1j0nkbt</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Recommendations for nail polish for beginners</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j0nkbt/recommendations_for_nail_polish_for_beginners/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1j0ngqq</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Easier gel couture top coat + thinner</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j0ngqq/easier_gel_couture_top_coat_thinner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1j0nesc</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Red ❤️</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vj2gey8y8zle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1j0n2tk</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Clionadh Cosmetics Macbeth</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0n2tk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1j0n0ov</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>I don't like them, they looked very strange to me, right?</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ltjx6pff5zle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1j0mpku</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>running up that hill ✨</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0mpku</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1j0miai</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Project Polish - Update 1</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0miai</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1j0memw</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Dupe for Fancy Gloss Tiffany?</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q719bbd10zle1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1j0lw8s</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>ILNP FTW!</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cmj5k2nkvyle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1j0liz0</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Why am I getting major bubbles using my mooncat speed demon top coat?</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j0liz0/why_am_i_getting_major_bubbles_using_my_mooncat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1j0las4</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Finally Bought the Horseshoe Magnet 🧲</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0las4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1j0l52c</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Disappointed</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0l52c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1j0kgtf</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Thoughts on new Cirque Colors collection Angel baby?</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wia9e9g1kyle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1j0kepa</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Nail Polish dice! But what color to ink the numbers?</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qsq4wuhkjyle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1j0k5wn</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>I'll get my lacquer -- tariffs be damned! 🍁🦅</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j0k5wn/ill_get_my_lacquer_tariffs_be_damned/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1j0k3ka</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>My Bees Knees Lacquer sale order came!✨️🥰</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0k3ka</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1j0jsk5</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>BKL The Celestial Kingdom ✨️🩵</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0jsk5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1j0jq3k</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>stunning starrily and lyn B</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0jq3k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1j0j5y4</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>coffee + starrily = love</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ukuglmve9yle1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1j0j2lc</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Gutted. What happened to BeautyGarde??</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/at8p6pnw8yle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1j0iv77</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Looking for a "Jelly Nail" UV Nail Polish</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j0iv77/looking_for_a_jelly_nail_uv_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1j0idum</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Death Valley Nails - Redemption Arc</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/glgrs1kk3yle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1j0i1fd</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>February Manis 💝</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0i1fd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1j0hpoy</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>🩷 Painted Polish pink crelly skittle for the last day of February 🩷</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qcvri3efyxle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1j0hoq2</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Flower Child might be my favorite polish I own currently! 🌸💙</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0hoq2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1j0hn5b</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Clionadh Norpsilocin</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/eh9bb34vxxle1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1j0hcl1</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>15 days of giveaways</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j0hcl1/15_days_of_giveaways/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1j0hay2</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>ISO color dupe</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ddy6ji5avxle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1j0guhj</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>PPU Comparison: GLL Come Again vs PFD Salamándra</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0guhj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1j0fdoa</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>She GLOWS</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0fdoa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1j0dxwz</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Sometimes I don't have the energy for fussy polishes</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ame267s5xle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1j0dk62</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Question about BKL’s “redacted” polishes</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j0dk62/question_about_bkls_redacted_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1j0davj</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Just Bitten by ORLY on natural nails 🩸🧛</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0davj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1j0d2x0</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>I finally got a decent video! Love Bites + Tiny Dancer</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/em833bqbzwle1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1j0ceyh</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>It’s On…</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0ceyh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1j0c05h</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Allergy Question</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j0c05h/allergy_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1j0b78v</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Is this achievable without gel?</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0b78v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1j0avzz</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Sometimes thermals are worth it</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0avzz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1j0assu</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Norpsilocin using my new magnet!</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0assu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1j09gd4</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>This thermal showing me my circulation issues</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gipyg2gj8wle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1j08jkp</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Not perfect but purrfect ;)</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j08jkp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1j08eqm</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Daisy Chain Polish 'Frost Flower'</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sjm80d3xzvle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1j07l5u</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Colores de Carol: Love is... a mystery (thermal)</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j07l5u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1j06u6e</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>OBSESSED with this magnetic, I cannot stop staring</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j06u6e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1j06h5c</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>february round up and polish bingo 💛</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j06h5c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1j06fy1</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Seche Restore</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j06fy1/seche_restore/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1j04n6c</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Does tiny dancer by cirque look so sparkly irl or just on camera?</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j04n6c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1j0u62b</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>My favorite effect😍😍😍</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hwszjki471me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1j0pwp3</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Weird pattern appearing on nail after top coats??</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/prxrb63hwzle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1j0oqwq</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Dr. Seuss Cat in the Hat Nails</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0oqwq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1j0m4ct</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>My new set of acrylics :)</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0m4ct</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1j0kprj</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>💥 Stranger Things 💥</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0kprj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1j0jnpa</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Is this in poor taste? lol</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0jnpa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1j0irdp</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Trying to decide which to do for my upcoming vacation, opinions??</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0irdp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1j0gwup</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>My first attempt at nail art</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sz244jt9sxle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1j0go1c</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>music festival nails!!</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f2tv61ggqxle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1j0fk78</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>How to achieve this set?</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/krbf42tzhxle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1j0dsir</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>New Set!!</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0dsir</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1j0drr1</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>what would you call this set?</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0drr1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1j0bqwt</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>I did a new set!</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0bqwt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1j0aac2</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Alexander McQueen Nails!💀</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lapzr50yewle1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1j09g21</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>How do you think the base color was done? One of my clients sent me this Inspo pic and I want to recreate it for her.</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qresrmng8wle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1j08nut</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>My favorite set I’ve done on myself</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j08nut</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1izwbhq</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>What can I improve?😊</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bw5q9cphasle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1j06k5f</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Always summer💓</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xr6h5t26jvle1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1j03nip</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Spring colors manicure</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j03nip</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Mar  2 08:09:25 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_03_02.xlsx
+++ b/data/collected_data/2025_03_02.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1229"/>
+  <dimension ref="A1:C1421"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21326,6 +21326,3270 @@
         </is>
       </c>
     </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1j1k81d</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Ideas for natural nails</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1k81d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1j1ky8y</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Help me pick my next set !</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1ky8y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1j1l3p4</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Red manis make me feel like I can take over the world</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1l3p4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1j1l0zs</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Is this removable skin, or is it living skin?</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pc940hky58me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1j1kid1</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>st patrick’s day nails!</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1kid1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1j1jynj</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>y2k nails 🩷🦓</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hh1tk7vdt7me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1j1c7m7</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Pink Cherry Nails</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fu25r8llr5me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1j1cmce</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>First time using press ons, thoughts?</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1cmce</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1j1dsf7</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>March, but make it subtle</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1dsf7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1j1e7se</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Help I’m an idiot. How do gel nails work</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j1e7se/help_im_an_idiot_how_do_gel_nails_work/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1j1eq1b</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>I’m a bit late, but this was a Valentine’s Day inspired set I did on myself!</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1eq1b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1j1fop2</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Did nail tech do my cat eye wrong?</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1fop2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1j1gpt6</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>vacation nails for an earth sign</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xehus5ftv6me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1j1hhs0</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Am I screwed?</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9h0ywr9f37me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1j1i4gd</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>where to buy stuff for making press ons that arent temu?</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j1i4gd/where_to_buy_stuff_for_making_press_ons_that/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1j1i5do</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Anything I can do to fix this?</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1i5do</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1j1jl7z</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>After doing XL nails for so long this feels weird to me</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/eiid7sh6p7me1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1j1jg4a</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>I don’t sit in chairs. I make my own.</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1jg4a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1j1iqgi</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>I'm cutting my nails for the first time</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j1iqgi/im_cutting_my_nails_for_the_first_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1j1ic2m</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>My nail Tech is the Best</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ygyr8joxb7me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1j1hyus</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Press-ons I Recreated</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1hyus</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1j1hu4i</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>I thought it was a good idea but now I have mix feelings about it</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mdi7codx67me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1j1hrck</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Builder gel pastel rainbow stripes</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/847dyqr467me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1j1hq2t</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Some nails I did for my friends bridal shower!</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/56a3hcpr57me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1j1hlsg</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>So happy with my new set!</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1hlsg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1j1h8p2</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>I ❣️ my tech</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bvcah1cy07me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1j1h8fk</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Slowly getting better at my press on application!</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1h8fk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1j1gkb8</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>First time almond nails</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1gkb8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1j1g91i</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Sugar Bling nails 💕</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zmhvb8qer6me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1j1g44h</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Maybe an unpopular opinion but I love lipstick shape 😅</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1g44h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1j1g272</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Nails I’ve done recently on my client’s natural nails as a hard  gel nail tech</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1g272</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1j1fziw</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>my gf did my nails! 😎</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1fziw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1j1fw8b</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Matcha nails 🍵</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1fw8b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1j1fog4</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>My second try - soft polygel</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1fog4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1j1fkwv</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Soft and girly mood</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1fkwv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1j1ez6t</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Is this soak off? - west coast dips gel polish</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://westcoastdips.ca/products/blushing-bride?variant=42444316737785</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1j1evft</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>press ons from olive &amp; june</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c5x2o6wje6me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1j1epfh</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Fill today! [Duck Nails]</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1epfh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1j1einn</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Ok, I love the color and I’m very loyal to my nail tech. Please tell me the middle finger nail doesn’t look crooked?</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1einn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1j1ea2c</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Happy March- more cat nails!</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fd39ag4b96me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1j1e1ka</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>I got new manicure today</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/frkxgs1876me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1j1dz60</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>walk…no RUN to your local dollar store, full kit, glue included and tons of great styles :)</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x6fnmgnj66me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1j1dulq</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Game Day means Nail Day.</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1dulq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1j1dufx</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Fresh Gel X just hits different</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1dufx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1j1czp5</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Been trying to learn nail art</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kfzo9nt3y5me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1j1cul0</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Advice</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1cul0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1j1cl4i</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>should my nail look like this?</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1cl4i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1j1ceq2</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>New milky white nails</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m7p22wt9t5me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1j1caeo</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Hard to take a good picture of my attempt at stained glass nails</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u6xv8t3as5me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1j1b8zd</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Is this a hangnail or an issue with my nail bed matrix?</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1b8zd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1j1b76j</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Do you see this SET?! *Kanye voice</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qri61vagj5me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1j1b5l1</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Well yes 🔮🙆🏻‍♀️😚</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1b5l1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1j1b1v2</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Porcelain Nails</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u1razg8ai5me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1j1b0ii</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>rainbow cat eye first timer! ✨</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bkyct99zh5me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1j1avx5</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Does this shape fit my nails?</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1avx5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1j1a4kd</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Trying to get into press-ons.. do these look okay? Shaped and cut by me.</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1a4kd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1j1a1vm</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>first time doing nail art in about a year:)</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1a1vm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1j1a0w6</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Spring is in the air today 🌼</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g0dvp7vz95me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1j19ez5</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Bold start to March</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pelafzy255me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1j19evc</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>What is the best top coat for nails? 💅</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j19evc/what_is_the_best_top_coat_for_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1j18rm3</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>I did a spring birthday set for myself</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/svu9lf1wz4me1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1j18jfw</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Slavic folklore</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j18jfw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1j18gyn</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>First time really trying to grow out my nails, went for a sheer nude so I can still see them</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nox3jshjx4me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1j18bdn</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Green for Saint Patrick’s Day 💚</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bz2q4wocw4me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1j17w5j</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Springtime St. Patrick’s vibe  🌷🍀</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j17w5j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1j17rgb</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>New hand painted nails</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0vhx1it0s4me1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1j17iig</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Looking for recommendations for flat shaped full cover nails</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j17iig/looking_for_recommendations_for_flat_shaped_full/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1j17fpu</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/irmatw9kp4me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1j174y0</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>A few months of growth</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j174y0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1j15to2</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>nail newbie: freaking out a little!</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kxvidjo9d4me1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1j15vkx</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Nothing special</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wkurnvind4me1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1j15kc4</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Top coat on press ons</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j15kc4/top_coat_on_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1j15hvu</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Today is a purple day</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j15hvu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1j15hf6</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Tried some little flowers for spring!</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j15hf6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1j14ujx</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>What I got vs what I asked for. I’m torn on whether to go back or not.. nail inspo from Amazon.com</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j14ujx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1j15efu</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Too yellow?</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j15efu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1j15ban</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Gel Polish</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j15ban</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1j150ke</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Barbie Beverly Hills Fashions set</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j150ke</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1j14tnf</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>back to red nails</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fcqghj7q54me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1j14pew</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Builder gel that I'm not sure they did a good job with</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j14pew</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1j10o8o</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>How would I fix this?</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j10o8o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1j11s2t</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Abstract nails</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j11s2t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1j14jgt</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Manicurist vs Peel-Off base</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j14jgt/manicurist_vs_peeloff_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1j14ghg</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>First time getting gel nails done, how does it look?</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xam1v3sw24me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1j13yid</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>cat claws</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j13yid</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1j0w0ur</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>I am sad that sometimes my Customer nails not dry peoperly. What Can be the reason? :( my own manicure for myself to me always works…</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0w0ur</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1j13wkp</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Removing gel: tiny leftovers after using e-file</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lfxtr7ssy3me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1j13av0</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Louboutin Inspired</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j13av0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1j13quv</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>How bad are they :(</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j13quv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1j13qpa</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Manifesting spring</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j13qpa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1j137av</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Loving my red press-ons</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rugvzulit3me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1j12uzl</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Nail growth progress photo x</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j12uzl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1j12no6</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>new set! i love my tech</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j12no6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1j12lxl</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>First set after 3 month break. Love a good nude 💅🏼💕</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j12lxl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1j12cx8</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>This polish with a different shape?</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7hctebexm3me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1j11nj4</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>look at these press ons i got!</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j11nj4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1j11hic</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Hit or no hit ?</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bv8i2970g3me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1j11blt</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>Yay or nah?</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/me3ddd1pe3me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1j117lv</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>I always love a good black French 💅💅✨✨</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l2s00f7td3me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1j1148t</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>My boyfriend made my initial "N" on her nail fot our Valentine's Day</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1148t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1j1lsli</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>I quit gel. Need support!</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1lsli</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1j1lqot</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>My attempt at stained glass 💅</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tku5iw5se8me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1j1lesu</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>February manicures</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1lesu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1j1jt2x</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>Why did you all tell me about PPU?</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4hnp09vlr7me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1j1jiro</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>two things: tell me ur fave cuticle oil and let me know if you think constant manicure changing damages your nails!</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kqafnlifo7me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1j1jf3n</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>My New Favorite</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1jf3n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1j1j26l</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>Bottled Rage</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1j26l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1j1iv3b</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>💙Teal Heart Frenchies💚</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1iv3b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1j1iig2</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Accidental future mani combo</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1iig2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1j1idoe</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Glossiest, glassiest QDTC?</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j1idoe/glossiest_glassiest_qdtc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1j1hmn0</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>This week has been rough so I wore some pretty polish and went fishing</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1hmn0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1j1h27i</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>I heard we were posting car livery nails, THAT'S MY NICHE!</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1h27i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1j1gyhp</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>Pantone matching?</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yp6x2y18y6me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1j1guig</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>Support Ukraine 🇺🇦</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nghoqjo4x6me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1j1guao</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>regular nail polishes similar to this colour?</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1guao</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1j1gcix</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>You all know what it is</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1gcix</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1j1fkzt</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>My first EVER indie nail polish: ILNP’s Deep Space 🔭✨💜</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1fkzt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1j1f2cj</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Advice for impatient nailpolish lovers?</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/50uyqvfcg6me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1j1ebv1</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>How to destash bottles with fill lines?</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j1ebv1/how_to_destash_bottles_with_fill_lines/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1j1e793</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>Favorite spring colors/polishes if you’re not into pastel?</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ln92d8nm86me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1j1dl7k</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>medium neutral brown polishes?</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1dl7k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1j1dl50</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>This polish is MAGICAL</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1dl50</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1j1die4</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>February Mani Roundup 💅</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1die4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1j1dbhp</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>The Closest I’m Getting to “Spirit Fingers”</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m284ii9w06me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1j1d9lg</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>The obsession has begun…</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p1g5u29g06me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1j1cmxb</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>So beautiful in the sun!</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/twqpslz4v5me1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1j1cgd9</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>My nails in January and February 💗</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1cgd9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1j1cfw8</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>Manucurist "Active" products</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j1cfw8/manucurist_active_products/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1j1c24t</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>The least Christmassy polish with “Christmas” in its name…</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1c24t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1j1b4f3</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>A “manly-cure” ft Essie After School Boy Blazer</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4izalbiui5me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1j1atd1</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Comparison Request</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j1atd1/comparison_request/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1j1a1ca</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>Ever have a bad nail day?</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1a1ca</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1j1a15q</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>HT LLB + GT Experiment</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yfjlv1x1a5me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1j19ya6</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>Feb nails, first time using magnetic polishes</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j19ya6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1j19upf</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Flower Child really IS That Girl</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j19upf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1j18qzc</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>[PR*] Did you know that the shimmer in the Sweet Tooth* &amp; Peach Ring* from the new ILNP collection match Fairy Dust &amp; Bluebell? I just had to do a lazy gradient!</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cwh7jacoz4me1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1j18q2v</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Builder gel nails ... I'm disappointed</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j18q2v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1j189x3</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>How does this shade look so good in literally any lighting?</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j189x3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1j17kee</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>One ring to rule them all</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g8s39rgkq4me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1j17is4</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Have My Heart</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j17is4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1j17420</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>February Manis</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j17420</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1j173hv</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>the March of the Birthstone polishes continues</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j173hv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1j16rnz</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>February</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j16rnz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1j16r2o</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>Base and top coat?</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j16r2o/base_and_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1j16eov</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>My Favorite Classic / Older China Glaze polishes (Part 1) see comments for details!</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j16eov</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1j16abj</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>Why don’t nail salons use Essie?</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j16abj/why_dont_nail_salons_use_essie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1j16384</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>Stuck in Observation, but my nails are Unforgettable 💜 (TW: needles)</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j16384</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1j1605h</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>🪲✨JEWEL BEETLE JEWEL BEETLE✨ 🪲</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ka9x6zble4me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1j15wd5</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>True Greatness Lies Within by BKL</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j15wd5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1j15mem</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>February Roundup 💌</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j15mem</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1j15mb0</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>chrome shorties</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1brffibqb4me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1j157aa</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>We're All Mad Here 🎩</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j157aa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1j153u0</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>February Nails 💌</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j153u0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1j14vz7</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>February</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j14vz7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1j13fzi</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>All my February manis</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j13fzi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1j131kh</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>I don’t usually do reds but I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j131kh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1j12tcl</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>She’s a President🩷</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j12tcl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1j12sxd</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>February Manis 💕💅🏼</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j12sxd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1j12o9q</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>Norpsilocin and Psilocin 💙💚❤️💜🤎🧡💛🩵</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i6wdzp2ep3me1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1j12f8i</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>Manis of February ❤️</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j12f8i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1j11g2f</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>Surprised by how much I adore Supernova 🤩</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/20ej8tnof3me1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1j11egp</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>Hot Wheels!</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j11egp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1j116ry</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>Annnd back to staring at my nails 🤩</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j116ry</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1j10vqp</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>Nails for the new Red Bull !</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j10vqp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1j10c48</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>Pink with purple shimmer</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j10c48/pink_with_purple_shimmer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1j10by1</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>Cracked is such an accurate brand name. It’s that good.🥲</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j10by1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1j103vr</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>Clionadh Monarch</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ofslgcd843me1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1j0yd7p</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>What type of nail tips and nail glue should i buy?</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j0yd7p/what_type_of_nail_tips_and_nail_glue_should_i_buy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1j0y3qo</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>Matte Black Nails Look Grey?</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j0y3qo/matte_black_nails_look_grey/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1j0x37v</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>PPU Monthly Megathread</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j0x37v/ppu_monthly_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1j0wgmt</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>Looking for european gel stockist of non-eu gel brands</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mkeb0exk02me1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1j1kk9m</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>mmmm shiny</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x0iw1v9a08me1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1j1kh8l</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>test nails</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1kh8l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1j1iuai</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>How do I achieve this look?</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1iuai</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1j1h87t</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>first time doing nails and i’m quite proud tbh also any tips are v appreciated</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1h87t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1j1h3yk</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>I finally got my stickers, what do you think?</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j1gg2csnz6me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1j1h3dr</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>Do you like this color combination?</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1h3dr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1j1ghy8</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>Green Shamrock Nails</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g1oguhzrt6me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1j1gecy</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>Loved these so much</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iprfkl5ts6me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1j1g03x</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>my gf did my nails! 😎</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1g03x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1j1d4ub</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>Easter grass inspired</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1d4ub</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1j1c568</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>Getting back into it</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/un3yy941r5me1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1j18wrs</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>Royal Nails</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/03c7qnu015me1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1j18kb4</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>Slavic folklore</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j18kb4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1j171e1</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>Sets I did since July 2024 (bonus a set on my husband :D)</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j171e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1j16is0</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>MPA Advanced Painting Gel Neon Color Palette Review</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1j16is0/mpa_advanced_painting_gel_neon_color_palette/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1j15e4i</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>Nails+ Mimi</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j15e4i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1j151pp</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>Barbie Beverly Hills Fashions set</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j151pp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1j143nq</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>My nails &amp; the inspo</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j143nq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1j0vtzd</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t>What should I do for spring?</t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0vtzd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>1j0xkxg</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>First spring nails!</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j0xkxg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>1j0w9dk</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>Spring wildflowers</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/75a0djs1y1me1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>